<commit_message>
Changes on naming conventions
- Changed T and NT patient begin, with T_ and NT_
- Row Cpg_array now named Mean_beta-value
- Return % of C2-score
- C1-C2 classification column name changed to C2 Score
- Fused together CpG and Qualu classification columns into a single Epigenetic classification
</commit_message>
<xml_diff>
--- a/excel_template/template_blank.xlsx
+++ b/excel_template/template_blank.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\HB_app_fork\excel_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D58FE57E-DDC9-4E00-92B3-053CAA28F75E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B9EC1F-D5BE-44CE-8EAA-3F80A2CE6816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16320" yWindow="-4155" windowWidth="16440" windowHeight="28440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,21 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
-    <t>T1</t>
-  </si>
-  <si>
-    <t>T2</t>
-  </si>
-  <si>
-    <t>T3</t>
-  </si>
-  <si>
-    <t>NT1</t>
-  </si>
-  <si>
-    <t>NT2</t>
-  </si>
-  <si>
     <t>DLK1</t>
   </si>
   <si>
@@ -108,28 +93,43 @@
     <t>VIM</t>
   </si>
   <si>
-    <t>CpG_Array</t>
-  </si>
-  <si>
-    <t>T4</t>
-  </si>
-  <si>
-    <t>T5</t>
-  </si>
-  <si>
-    <t>NT3</t>
-  </si>
-  <si>
-    <t>NT4</t>
-  </si>
-  <si>
-    <t>NT5</t>
-  </si>
-  <si>
     <t>Biomarker</t>
   </si>
   <si>
     <t>PUMA_value</t>
+  </si>
+  <si>
+    <t>T_1</t>
+  </si>
+  <si>
+    <t>T_2</t>
+  </si>
+  <si>
+    <t>T_3</t>
+  </si>
+  <si>
+    <t>T_4</t>
+  </si>
+  <si>
+    <t>T_5</t>
+  </si>
+  <si>
+    <t>NT_1</t>
+  </si>
+  <si>
+    <t>NT_2</t>
+  </si>
+  <si>
+    <t>NT_3</t>
+  </si>
+  <si>
+    <t>NT_4</t>
+  </si>
+  <si>
+    <t>NT_5</t>
+  </si>
+  <si>
+    <t>Mean_beta-value</t>
   </si>
 </sst>
 </file>
@@ -538,144 +538,144 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomRight" activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -690,7 +690,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -705,27 +705,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MediaLengthInSeconds xmlns="b49300fb-5a15-41c5-a699-e56f15cf87c0" xsi:nil="true"/>
-    <TaxCatchAll xmlns="d6f5471d-30bd-463b-83c2-41c4d2d2dcf8" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b49300fb-5a15-41c5-a699-e56f15cf87c0">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101002398FB7092F00C4DB16FA976D26C2BCB" ma:contentTypeVersion="14" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="0d796344d46bbfc9e31274fe28d98393">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b49300fb-5a15-41c5-a699-e56f15cf87c0" xmlns:ns3="d6f5471d-30bd-463b-83c2-41c4d2d2dcf8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="154f4c8b679df23a2dd430078f701f0d" ns2:_="" ns3:_="">
     <xsd:import namespace="b49300fb-5a15-41c5-a699-e56f15cf87c0"/>
@@ -954,26 +933,28 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MediaLengthInSeconds xmlns="b49300fb-5a15-41c5-a699-e56f15cf87c0" xsi:nil="true"/>
+    <TaxCatchAll xmlns="d6f5471d-30bd-463b-83c2-41c4d2d2dcf8" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b49300fb-5a15-41c5-a699-e56f15cf87c0">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{313A6721-9CCD-4F80-B9F4-149EDF7B2021}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03433CC9-6300-4723-B65D-286A5E9F5923}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b49300fb-5a15-41c5-a699-e56f15cf87c0"/>
-    <ds:schemaRef ds:uri="d6f5471d-30bd-463b-83c2-41c4d2d2dcf8"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9019AD50-4732-4B34-AA33-87FF5B36AFF2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -990,4 +971,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03433CC9-6300-4723-B65D-286A5E9F5923}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b49300fb-5a15-41c5-a699-e56f15cf87c0"/>
+    <ds:schemaRef ds:uri="d6f5471d-30bd-463b-83c2-41c4d2d2dcf8"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{313A6721-9CCD-4F80-B9F4-149EDF7B2021}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>